<commit_message>
Fixed construction algorithm and added some excel data.
</commit_message>
<xml_diff>
--- a/FURI_Spring/FURI_Spring/FURI_Data/Homogeneous_Test_2.xlsx
+++ b/FURI_Spring/FURI_Spring/FURI_Data/Homogeneous_Test_2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke_\Desktop\FURI_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke_\Documents\GitHub\FURI\FURI_Spring\FURI_Spring\FURI_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDB885C-4DC7-4BA7-963C-3814228D14A7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8118" windowHeight="5772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8120" windowHeight="5773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homogeneous_Test_2" sheetId="1" r:id="rId1"/>
@@ -601,6 +602,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percentage of Homogeneous</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Arrays</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -858,7 +889,7 @@
         <c:axId val="724653904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -876,7 +907,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -978,6 +1009,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Homogeneous Arrays</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1734,6 +1790,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Homogeneous Arrays</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7522,16 +7603,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200660</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>94403</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>292101</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>60959</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7931,15 +8012,15 @@
   <dimension ref="A1:P421"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="6" max="6" width="16.05078125" customWidth="1"/>
+    <col min="6" max="6" width="16.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7986,7 +8067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>2</v>
       </c>
@@ -8034,7 +8115,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8082,7 +8163,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -8130,7 +8211,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>2</v>
       </c>
@@ -8178,7 +8259,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -8226,7 +8307,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>2</v>
       </c>
@@ -8274,7 +8355,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>2</v>
       </c>
@@ -8322,7 +8403,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>2</v>
       </c>
@@ -8370,7 +8451,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>2</v>
       </c>
@@ -8418,7 +8499,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>2</v>
       </c>
@@ -8466,7 +8547,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>2</v>
       </c>
@@ -8514,7 +8595,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>2</v>
       </c>
@@ -8562,7 +8643,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>2</v>
       </c>
@@ -8610,7 +8691,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>2</v>
       </c>
@@ -8658,7 +8739,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>2</v>
       </c>
@@ -8706,7 +8787,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>3</v>
       </c>
@@ -8754,7 +8835,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>3</v>
       </c>
@@ -8802,7 +8883,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>3</v>
       </c>
@@ -8850,7 +8931,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>3</v>
       </c>
@@ -8898,7 +8979,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>3</v>
       </c>
@@ -8946,7 +9027,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>3</v>
       </c>
@@ -8994,7 +9075,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>3</v>
       </c>
@@ -9042,7 +9123,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>3</v>
       </c>
@@ -9090,7 +9171,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>3</v>
       </c>
@@ -9138,7 +9219,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>3</v>
       </c>
@@ -9186,7 +9267,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>3</v>
       </c>
@@ -9234,7 +9315,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>3</v>
       </c>
@@ -9282,7 +9363,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>3</v>
       </c>
@@ -9330,7 +9411,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>3</v>
       </c>
@@ -9378,7 +9459,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>3</v>
       </c>
@@ -9426,7 +9507,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>4</v>
       </c>
@@ -9474,7 +9555,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>4</v>
       </c>
@@ -9522,7 +9603,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>4</v>
       </c>
@@ -9570,7 +9651,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>4</v>
       </c>
@@ -9618,7 +9699,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>4</v>
       </c>
@@ -9666,7 +9747,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>4</v>
       </c>
@@ -9714,7 +9795,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>4</v>
       </c>
@@ -9762,7 +9843,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>4</v>
       </c>
@@ -9810,7 +9891,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>4</v>
       </c>
@@ -9833,7 +9914,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>4</v>
       </c>
@@ -9856,7 +9937,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>4</v>
       </c>
@@ -9879,7 +9960,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>4</v>
       </c>
@@ -9902,7 +9983,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>4</v>
       </c>
@@ -9925,7 +10006,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>4</v>
       </c>
@@ -9948,7 +10029,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>4</v>
       </c>
@@ -9971,7 +10052,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>5</v>
       </c>
@@ -9994,7 +10075,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>5</v>
       </c>
@@ -10017,7 +10098,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>5</v>
       </c>
@@ -10040,7 +10121,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>5</v>
       </c>
@@ -10063,7 +10144,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>5</v>
       </c>
@@ -10086,7 +10167,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>5</v>
       </c>
@@ -10109,7 +10190,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>5</v>
       </c>
@@ -10132,7 +10213,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>5</v>
       </c>
@@ -10155,7 +10236,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>5</v>
       </c>
@@ -10178,7 +10259,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>5</v>
       </c>
@@ -10201,7 +10282,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>5</v>
       </c>
@@ -10224,7 +10305,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>5</v>
       </c>
@@ -10247,7 +10328,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>5</v>
       </c>
@@ -10270,7 +10351,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>5</v>
       </c>
@@ -10293,7 +10374,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>5</v>
       </c>
@@ -10316,7 +10397,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>6</v>
       </c>
@@ -10339,7 +10420,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>6</v>
       </c>
@@ -10362,7 +10443,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>6</v>
       </c>
@@ -10385,7 +10466,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>6</v>
       </c>
@@ -10408,7 +10489,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>6</v>
       </c>
@@ -10431,7 +10512,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>6</v>
       </c>
@@ -10454,7 +10535,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>6</v>
       </c>
@@ -10477,7 +10558,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>6</v>
       </c>
@@ -10500,7 +10581,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>6</v>
       </c>
@@ -10523,7 +10604,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>6</v>
       </c>
@@ -10546,7 +10627,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>6</v>
       </c>
@@ -10569,7 +10650,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>6</v>
       </c>
@@ -10592,7 +10673,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>6</v>
       </c>
@@ -10615,7 +10696,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>6</v>
       </c>
@@ -10638,7 +10719,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>6</v>
       </c>
@@ -10661,7 +10742,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>7</v>
       </c>
@@ -10684,7 +10765,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>7</v>
       </c>
@@ -10707,7 +10788,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>7</v>
       </c>
@@ -10730,7 +10811,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A80">
         <v>7</v>
       </c>
@@ -10753,7 +10834,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A81">
         <v>7</v>
       </c>
@@ -10776,7 +10857,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>7</v>
       </c>
@@ -10799,7 +10880,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>7</v>
       </c>
@@ -10822,7 +10903,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>7</v>
       </c>
@@ -10845,7 +10926,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>7</v>
       </c>
@@ -10868,7 +10949,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A86">
         <v>7</v>
       </c>
@@ -10891,7 +10972,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A87">
         <v>7</v>
       </c>
@@ -10914,7 +10995,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A88">
         <v>7</v>
       </c>
@@ -10937,7 +11018,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A89">
         <v>7</v>
       </c>
@@ -10960,7 +11041,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A90">
         <v>7</v>
       </c>
@@ -10983,7 +11064,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A91">
         <v>7</v>
       </c>
@@ -11006,7 +11087,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A92">
         <v>8</v>
       </c>
@@ -11029,7 +11110,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A93">
         <v>8</v>
       </c>
@@ -11052,7 +11133,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A94">
         <v>8</v>
       </c>
@@ -11075,7 +11156,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A95">
         <v>8</v>
       </c>
@@ -11098,7 +11179,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A96">
         <v>8</v>
       </c>
@@ -11121,7 +11202,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A97">
         <v>8</v>
       </c>
@@ -11144,7 +11225,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A98">
         <v>8</v>
       </c>
@@ -11167,7 +11248,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A99">
         <v>8</v>
       </c>
@@ -11190,7 +11271,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A100">
         <v>8</v>
       </c>
@@ -11213,7 +11294,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A101">
         <v>8</v>
       </c>
@@ -11236,7 +11317,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A102">
         <v>8</v>
       </c>
@@ -11259,7 +11340,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A103">
         <v>8</v>
       </c>
@@ -11282,7 +11363,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A104">
         <v>8</v>
       </c>
@@ -11305,7 +11386,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A105">
         <v>8</v>
       </c>
@@ -11328,7 +11409,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A106">
         <v>8</v>
       </c>
@@ -11351,7 +11432,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A107">
         <v>9</v>
       </c>
@@ -11374,7 +11455,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A108">
         <v>9</v>
       </c>
@@ -11397,7 +11478,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A109">
         <v>9</v>
       </c>
@@ -11420,7 +11501,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A110">
         <v>9</v>
       </c>
@@ -11443,7 +11524,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A111">
         <v>9</v>
       </c>
@@ -11466,7 +11547,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A112">
         <v>9</v>
       </c>
@@ -11489,7 +11570,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A113">
         <v>9</v>
       </c>
@@ -11512,7 +11593,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A114">
         <v>9</v>
       </c>
@@ -11535,7 +11616,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A115">
         <v>9</v>
       </c>
@@ -11558,7 +11639,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A116">
         <v>9</v>
       </c>
@@ -11581,7 +11662,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A117">
         <v>9</v>
       </c>
@@ -11604,7 +11685,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A118">
         <v>9</v>
       </c>
@@ -11627,7 +11708,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A119">
         <v>9</v>
       </c>
@@ -11650,7 +11731,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A120">
         <v>9</v>
       </c>
@@ -11673,7 +11754,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A121">
         <v>9</v>
       </c>
@@ -11696,7 +11777,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A122">
         <v>10</v>
       </c>
@@ -11719,7 +11800,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A123">
         <v>10</v>
       </c>
@@ -11742,7 +11823,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A124">
         <v>10</v>
       </c>
@@ -11765,7 +11846,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A125">
         <v>10</v>
       </c>
@@ -11788,7 +11869,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A126">
         <v>10</v>
       </c>
@@ -11811,7 +11892,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A127">
         <v>10</v>
       </c>
@@ -11834,7 +11915,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A128">
         <v>10</v>
       </c>
@@ -11857,7 +11938,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A129">
         <v>10</v>
       </c>
@@ -11880,7 +11961,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A130">
         <v>10</v>
       </c>
@@ -11903,7 +11984,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A131">
         <v>10</v>
       </c>
@@ -11926,7 +12007,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A132">
         <v>10</v>
       </c>
@@ -11949,7 +12030,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A133">
         <v>10</v>
       </c>
@@ -11972,7 +12053,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A134">
         <v>10</v>
       </c>
@@ -11995,7 +12076,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A135">
         <v>10</v>
       </c>
@@ -12018,7 +12099,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A136">
         <v>10</v>
       </c>
@@ -12041,7 +12122,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A137">
         <v>11</v>
       </c>
@@ -12064,7 +12145,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A138">
         <v>11</v>
       </c>
@@ -12087,7 +12168,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A139">
         <v>11</v>
       </c>
@@ -12110,7 +12191,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A140">
         <v>11</v>
       </c>
@@ -12133,7 +12214,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A141">
         <v>11</v>
       </c>
@@ -12156,7 +12237,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A142">
         <v>11</v>
       </c>
@@ -12179,7 +12260,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A143">
         <v>11</v>
       </c>
@@ -12202,7 +12283,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A144">
         <v>11</v>
       </c>
@@ -12225,7 +12306,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A145">
         <v>11</v>
       </c>
@@ -12248,7 +12329,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A146">
         <v>11</v>
       </c>
@@ -12271,7 +12352,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A147">
         <v>11</v>
       </c>
@@ -12294,7 +12375,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A148">
         <v>11</v>
       </c>
@@ -12317,7 +12398,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A149">
         <v>11</v>
       </c>
@@ -12340,7 +12421,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A150">
         <v>11</v>
       </c>
@@ -12363,7 +12444,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A151">
         <v>11</v>
       </c>
@@ -12386,7 +12467,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A152">
         <v>12</v>
       </c>
@@ -12409,7 +12490,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A153">
         <v>12</v>
       </c>
@@ -12432,7 +12513,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A154">
         <v>12</v>
       </c>
@@ -12455,7 +12536,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A155">
         <v>12</v>
       </c>
@@ -12478,7 +12559,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A156">
         <v>12</v>
       </c>
@@ -12501,7 +12582,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A157">
         <v>12</v>
       </c>
@@ -12524,7 +12605,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A158">
         <v>12</v>
       </c>
@@ -12547,7 +12628,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A159">
         <v>12</v>
       </c>
@@ -12570,7 +12651,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A160">
         <v>12</v>
       </c>
@@ -12593,7 +12674,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A161">
         <v>12</v>
       </c>
@@ -12616,7 +12697,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A162">
         <v>12</v>
       </c>
@@ -12639,7 +12720,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A163">
         <v>12</v>
       </c>
@@ -12662,7 +12743,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A164">
         <v>12</v>
       </c>
@@ -12685,7 +12766,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A165">
         <v>12</v>
       </c>
@@ -12708,7 +12789,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A166">
         <v>12</v>
       </c>
@@ -12731,7 +12812,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A167">
         <v>13</v>
       </c>
@@ -12754,7 +12835,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A168">
         <v>13</v>
       </c>
@@ -12777,7 +12858,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A169">
         <v>13</v>
       </c>
@@ -12800,7 +12881,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A170">
         <v>13</v>
       </c>
@@ -12823,7 +12904,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A171">
         <v>13</v>
       </c>
@@ -12846,7 +12927,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A172">
         <v>13</v>
       </c>
@@ -12869,7 +12950,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A173">
         <v>13</v>
       </c>
@@ -12892,7 +12973,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A174">
         <v>13</v>
       </c>
@@ -12915,7 +12996,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A175">
         <v>13</v>
       </c>
@@ -12938,7 +13019,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A176">
         <v>13</v>
       </c>
@@ -12961,7 +13042,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A177">
         <v>13</v>
       </c>
@@ -12984,7 +13065,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A178">
         <v>13</v>
       </c>
@@ -13007,7 +13088,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A179">
         <v>13</v>
       </c>
@@ -13030,7 +13111,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A180">
         <v>13</v>
       </c>
@@ -13053,7 +13134,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A181">
         <v>13</v>
       </c>
@@ -13076,7 +13157,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A182">
         <v>14</v>
       </c>
@@ -13099,7 +13180,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A183">
         <v>14</v>
       </c>
@@ -13122,7 +13203,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A184">
         <v>14</v>
       </c>
@@ -13145,7 +13226,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A185">
         <v>14</v>
       </c>
@@ -13168,7 +13249,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A186">
         <v>14</v>
       </c>
@@ -13191,7 +13272,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A187">
         <v>14</v>
       </c>
@@ -13214,7 +13295,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A188">
         <v>14</v>
       </c>
@@ -13237,7 +13318,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A189">
         <v>14</v>
       </c>
@@ -13260,7 +13341,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A190">
         <v>14</v>
       </c>
@@ -13283,7 +13364,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A191">
         <v>14</v>
       </c>
@@ -13306,7 +13387,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A192">
         <v>14</v>
       </c>
@@ -13329,7 +13410,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A193">
         <v>14</v>
       </c>
@@ -13352,7 +13433,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A194">
         <v>14</v>
       </c>
@@ -13375,7 +13456,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A195">
         <v>14</v>
       </c>
@@ -13398,7 +13479,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A196">
         <v>14</v>
       </c>
@@ -13421,7 +13502,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A197">
         <v>15</v>
       </c>
@@ -13444,7 +13525,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A198">
         <v>15</v>
       </c>
@@ -13467,7 +13548,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A199">
         <v>15</v>
       </c>
@@ -13490,7 +13571,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A200">
         <v>15</v>
       </c>
@@ -13513,7 +13594,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A201">
         <v>15</v>
       </c>
@@ -13536,7 +13617,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A202">
         <v>15</v>
       </c>
@@ -13559,7 +13640,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A203">
         <v>15</v>
       </c>
@@ -13582,7 +13663,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A204">
         <v>15</v>
       </c>
@@ -13605,7 +13686,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A205">
         <v>15</v>
       </c>
@@ -13628,7 +13709,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A206">
         <v>15</v>
       </c>
@@ -13651,7 +13732,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A207">
         <v>15</v>
       </c>
@@ -13674,7 +13755,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A208">
         <v>15</v>
       </c>
@@ -13697,7 +13778,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A209">
         <v>15</v>
       </c>
@@ -13720,7 +13801,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A210">
         <v>15</v>
       </c>
@@ -13743,7 +13824,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A211">
         <v>15</v>
       </c>
@@ -13766,7 +13847,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A212">
         <v>16</v>
       </c>
@@ -13789,7 +13870,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A213">
         <v>16</v>
       </c>
@@ -13812,7 +13893,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A214">
         <v>16</v>
       </c>
@@ -13835,7 +13916,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A215">
         <v>16</v>
       </c>
@@ -13858,7 +13939,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A216">
         <v>16</v>
       </c>
@@ -13881,7 +13962,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A217">
         <v>16</v>
       </c>
@@ -13904,7 +13985,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A218">
         <v>16</v>
       </c>
@@ -13927,7 +14008,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A219">
         <v>16</v>
       </c>
@@ -13950,7 +14031,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A220">
         <v>16</v>
       </c>
@@ -13973,7 +14054,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A221">
         <v>16</v>
       </c>
@@ -13996,7 +14077,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A222">
         <v>16</v>
       </c>
@@ -14019,7 +14100,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A223">
         <v>16</v>
       </c>
@@ -14042,7 +14123,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A224">
         <v>16</v>
       </c>
@@ -14065,7 +14146,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A225">
         <v>16</v>
       </c>
@@ -14088,7 +14169,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A226">
         <v>16</v>
       </c>
@@ -14111,7 +14192,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A227">
         <v>17</v>
       </c>
@@ -14134,7 +14215,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A228">
         <v>17</v>
       </c>
@@ -14157,7 +14238,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A229">
         <v>17</v>
       </c>
@@ -14180,7 +14261,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A230">
         <v>17</v>
       </c>
@@ -14203,7 +14284,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A231">
         <v>17</v>
       </c>
@@ -14226,7 +14307,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A232">
         <v>17</v>
       </c>
@@ -14249,7 +14330,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A233">
         <v>17</v>
       </c>
@@ -14272,7 +14353,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A234">
         <v>17</v>
       </c>
@@ -14295,7 +14376,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A235">
         <v>17</v>
       </c>
@@ -14318,7 +14399,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A236">
         <v>17</v>
       </c>
@@ -14341,7 +14422,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A237">
         <v>17</v>
       </c>
@@ -14364,7 +14445,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A238">
         <v>17</v>
       </c>
@@ -14387,7 +14468,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A239">
         <v>17</v>
       </c>
@@ -14410,7 +14491,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A240">
         <v>17</v>
       </c>
@@ -14433,7 +14514,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A241">
         <v>17</v>
       </c>
@@ -14456,7 +14537,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A242">
         <v>18</v>
       </c>
@@ -14479,7 +14560,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A243">
         <v>18</v>
       </c>
@@ -14502,7 +14583,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A244">
         <v>18</v>
       </c>
@@ -14525,7 +14606,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A245">
         <v>18</v>
       </c>
@@ -14548,7 +14629,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A246">
         <v>18</v>
       </c>
@@ -14571,7 +14652,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A247">
         <v>18</v>
       </c>
@@ -14594,7 +14675,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A248">
         <v>18</v>
       </c>
@@ -14617,7 +14698,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A249">
         <v>18</v>
       </c>
@@ -14640,7 +14721,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A250">
         <v>18</v>
       </c>
@@ -14663,7 +14744,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A251">
         <v>18</v>
       </c>
@@ -14686,7 +14767,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A252">
         <v>18</v>
       </c>
@@ -14709,7 +14790,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A253">
         <v>18</v>
       </c>
@@ -14732,7 +14813,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A254">
         <v>18</v>
       </c>
@@ -14755,7 +14836,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A255">
         <v>18</v>
       </c>
@@ -14778,7 +14859,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A256">
         <v>18</v>
       </c>
@@ -14801,7 +14882,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A257">
         <v>19</v>
       </c>
@@ -14824,7 +14905,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A258">
         <v>19</v>
       </c>
@@ -14847,7 +14928,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A259">
         <v>19</v>
       </c>
@@ -14870,7 +14951,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A260">
         <v>19</v>
       </c>
@@ -14893,7 +14974,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A261">
         <v>19</v>
       </c>
@@ -14916,7 +14997,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A262">
         <v>19</v>
       </c>
@@ -14939,7 +15020,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A263">
         <v>19</v>
       </c>
@@ -14962,7 +15043,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A264">
         <v>19</v>
       </c>
@@ -14985,7 +15066,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A265">
         <v>19</v>
       </c>
@@ -15008,7 +15089,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A266">
         <v>19</v>
       </c>
@@ -15031,7 +15112,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A267">
         <v>19</v>
       </c>
@@ -15054,7 +15135,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A268">
         <v>19</v>
       </c>
@@ -15077,7 +15158,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A269">
         <v>19</v>
       </c>
@@ -15100,7 +15181,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A270">
         <v>19</v>
       </c>
@@ -15123,7 +15204,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A271">
         <v>19</v>
       </c>
@@ -15146,7 +15227,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A272">
         <v>20</v>
       </c>
@@ -15169,7 +15250,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A273">
         <v>20</v>
       </c>
@@ -15192,7 +15273,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A274">
         <v>20</v>
       </c>
@@ -15215,7 +15296,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A275">
         <v>20</v>
       </c>
@@ -15238,7 +15319,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A276">
         <v>20</v>
       </c>
@@ -15261,7 +15342,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A277">
         <v>20</v>
       </c>
@@ -15284,7 +15365,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A278">
         <v>20</v>
       </c>
@@ -15307,7 +15388,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A279">
         <v>20</v>
       </c>
@@ -15330,7 +15411,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A280">
         <v>20</v>
       </c>
@@ -15353,7 +15434,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A281">
         <v>20</v>
       </c>
@@ -15376,7 +15457,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A282">
         <v>20</v>
       </c>
@@ -15399,7 +15480,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A283">
         <v>20</v>
       </c>
@@ -15422,7 +15503,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A284">
         <v>20</v>
       </c>
@@ -15445,7 +15526,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A285">
         <v>20</v>
       </c>
@@ -15468,7 +15549,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A286">
         <v>20</v>
       </c>
@@ -15491,7 +15572,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A287">
         <v>21</v>
       </c>
@@ -15514,7 +15595,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A288">
         <v>21</v>
       </c>
@@ -15537,7 +15618,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A289">
         <v>21</v>
       </c>
@@ -15560,7 +15641,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A290">
         <v>21</v>
       </c>
@@ -15583,7 +15664,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A291">
         <v>21</v>
       </c>
@@ -15606,7 +15687,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A292">
         <v>21</v>
       </c>
@@ -15629,7 +15710,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A293">
         <v>21</v>
       </c>
@@ -15652,7 +15733,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A294">
         <v>21</v>
       </c>
@@ -15675,7 +15756,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A295">
         <v>21</v>
       </c>
@@ -15698,7 +15779,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A296">
         <v>21</v>
       </c>
@@ -15721,7 +15802,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A297">
         <v>21</v>
       </c>
@@ -15744,7 +15825,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A298">
         <v>21</v>
       </c>
@@ -15767,7 +15848,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A299">
         <v>21</v>
       </c>
@@ -15790,7 +15871,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A300">
         <v>21</v>
       </c>
@@ -15813,7 +15894,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A301">
         <v>21</v>
       </c>
@@ -15836,7 +15917,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A302">
         <v>22</v>
       </c>
@@ -15859,7 +15940,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A303">
         <v>22</v>
       </c>
@@ -15882,7 +15963,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A304">
         <v>22</v>
       </c>
@@ -15905,7 +15986,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A305">
         <v>22</v>
       </c>
@@ -15928,7 +16009,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A306">
         <v>22</v>
       </c>
@@ -15951,7 +16032,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A307">
         <v>22</v>
       </c>
@@ -15974,7 +16055,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A308">
         <v>22</v>
       </c>
@@ -15997,7 +16078,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A309">
         <v>22</v>
       </c>
@@ -16020,7 +16101,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A310">
         <v>22</v>
       </c>
@@ -16043,7 +16124,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A311">
         <v>22</v>
       </c>
@@ -16066,7 +16147,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A312">
         <v>22</v>
       </c>
@@ -16089,7 +16170,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A313">
         <v>22</v>
       </c>
@@ -16112,7 +16193,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A314">
         <v>22</v>
       </c>
@@ -16135,7 +16216,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A315">
         <v>22</v>
       </c>
@@ -16158,7 +16239,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A316">
         <v>22</v>
       </c>
@@ -16181,7 +16262,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A317">
         <v>23</v>
       </c>
@@ -16204,7 +16285,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A318">
         <v>23</v>
       </c>
@@ -16227,7 +16308,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A319">
         <v>23</v>
       </c>
@@ -16250,7 +16331,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A320">
         <v>23</v>
       </c>
@@ -16273,7 +16354,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A321">
         <v>23</v>
       </c>
@@ -16296,7 +16377,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A322">
         <v>23</v>
       </c>
@@ -16319,7 +16400,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A323">
         <v>23</v>
       </c>
@@ -16342,7 +16423,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A324">
         <v>23</v>
       </c>
@@ -16365,7 +16446,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A325">
         <v>23</v>
       </c>
@@ -16388,7 +16469,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A326">
         <v>23</v>
       </c>
@@ -16411,7 +16492,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A327">
         <v>23</v>
       </c>
@@ -16434,7 +16515,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A328">
         <v>23</v>
       </c>
@@ -16457,7 +16538,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A329">
         <v>23</v>
       </c>
@@ -16480,7 +16561,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A330">
         <v>23</v>
       </c>
@@ -16503,7 +16584,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A331">
         <v>23</v>
       </c>
@@ -16526,7 +16607,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A332">
         <v>24</v>
       </c>
@@ -16549,7 +16630,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A333">
         <v>24</v>
       </c>
@@ -16572,7 +16653,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="334" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A334">
         <v>24</v>
       </c>
@@ -16595,7 +16676,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A335">
         <v>24</v>
       </c>
@@ -16618,7 +16699,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A336">
         <v>24</v>
       </c>
@@ -16641,7 +16722,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A337">
         <v>24</v>
       </c>
@@ -16664,7 +16745,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A338">
         <v>24</v>
       </c>
@@ -16687,7 +16768,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A339">
         <v>24</v>
       </c>
@@ -16710,7 +16791,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A340">
         <v>24</v>
       </c>
@@ -16733,7 +16814,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A341">
         <v>24</v>
       </c>
@@ -16756,7 +16837,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A342">
         <v>24</v>
       </c>
@@ -16779,7 +16860,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A343">
         <v>24</v>
       </c>
@@ -16802,7 +16883,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A344">
         <v>24</v>
       </c>
@@ -16825,7 +16906,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A345">
         <v>24</v>
       </c>
@@ -16848,7 +16929,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A346">
         <v>24</v>
       </c>
@@ -16871,7 +16952,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A347">
         <v>25</v>
       </c>
@@ -16894,7 +16975,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A348">
         <v>25</v>
       </c>
@@ -16917,7 +16998,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A349">
         <v>25</v>
       </c>
@@ -16940,7 +17021,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A350">
         <v>25</v>
       </c>
@@ -16963,7 +17044,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A351">
         <v>25</v>
       </c>
@@ -16986,7 +17067,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A352">
         <v>25</v>
       </c>
@@ -17009,7 +17090,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A353">
         <v>25</v>
       </c>
@@ -17032,7 +17113,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A354">
         <v>25</v>
       </c>
@@ -17055,7 +17136,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A355">
         <v>25</v>
       </c>
@@ -17078,7 +17159,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A356">
         <v>25</v>
       </c>
@@ -17101,7 +17182,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A357">
         <v>25</v>
       </c>
@@ -17124,7 +17205,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A358">
         <v>25</v>
       </c>
@@ -17147,7 +17228,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A359">
         <v>25</v>
       </c>
@@ -17170,7 +17251,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A360">
         <v>25</v>
       </c>
@@ -17193,7 +17274,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A361">
         <v>25</v>
       </c>
@@ -17216,7 +17297,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A362">
         <v>26</v>
       </c>
@@ -17239,7 +17320,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A363">
         <v>26</v>
       </c>
@@ -17262,7 +17343,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A364">
         <v>26</v>
       </c>
@@ -17285,7 +17366,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A365">
         <v>26</v>
       </c>
@@ -17308,7 +17389,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A366">
         <v>26</v>
       </c>
@@ -17331,7 +17412,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A367">
         <v>26</v>
       </c>
@@ -17354,7 +17435,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A368">
         <v>26</v>
       </c>
@@ -17377,7 +17458,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A369">
         <v>26</v>
       </c>
@@ -17400,7 +17481,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A370">
         <v>26</v>
       </c>
@@ -17423,7 +17504,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A371">
         <v>26</v>
       </c>
@@ -17446,7 +17527,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A372">
         <v>26</v>
       </c>
@@ -17469,7 +17550,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A373">
         <v>26</v>
       </c>
@@ -17492,7 +17573,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A374">
         <v>26</v>
       </c>
@@ -17515,7 +17596,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A375">
         <v>26</v>
       </c>
@@ -17538,7 +17619,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A376">
         <v>26</v>
       </c>
@@ -17561,7 +17642,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A377">
         <v>27</v>
       </c>
@@ -17584,7 +17665,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A378">
         <v>27</v>
       </c>
@@ -17607,7 +17688,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="379" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A379">
         <v>27</v>
       </c>
@@ -17630,7 +17711,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="380" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A380">
         <v>27</v>
       </c>
@@ -17653,7 +17734,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="381" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A381">
         <v>27</v>
       </c>
@@ -17676,7 +17757,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="382" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A382">
         <v>27</v>
       </c>
@@ -17699,7 +17780,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="383" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A383">
         <v>27</v>
       </c>
@@ -17722,7 +17803,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="384" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A384">
         <v>27</v>
       </c>
@@ -17745,7 +17826,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="385" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A385">
         <v>27</v>
       </c>
@@ -17768,7 +17849,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="386" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A386">
         <v>27</v>
       </c>
@@ -17791,7 +17872,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="387" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A387">
         <v>27</v>
       </c>
@@ -17814,7 +17895,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="388" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A388">
         <v>27</v>
       </c>
@@ -17837,7 +17918,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="389" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A389">
         <v>27</v>
       </c>
@@ -17860,7 +17941,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="390" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A390">
         <v>27</v>
       </c>
@@ -17883,7 +17964,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="391" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A391">
         <v>27</v>
       </c>
@@ -17906,7 +17987,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="392" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A392">
         <v>28</v>
       </c>
@@ -17929,7 +18010,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="393" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A393">
         <v>28</v>
       </c>
@@ -17952,7 +18033,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="394" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="394" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A394">
         <v>28</v>
       </c>
@@ -17975,7 +18056,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="395" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A395">
         <v>28</v>
       </c>
@@ -17998,7 +18079,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="396" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A396">
         <v>28</v>
       </c>
@@ -18021,7 +18102,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="397" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A397">
         <v>28</v>
       </c>
@@ -18044,7 +18125,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="398" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A398">
         <v>28</v>
       </c>
@@ -18067,7 +18148,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="399" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A399">
         <v>28</v>
       </c>
@@ -18090,7 +18171,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="400" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A400">
         <v>28</v>
       </c>
@@ -18113,7 +18194,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="401" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A401">
         <v>28</v>
       </c>
@@ -18136,7 +18217,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="402" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A402">
         <v>28</v>
       </c>
@@ -18159,7 +18240,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="403" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="403" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A403">
         <v>28</v>
       </c>
@@ -18182,7 +18263,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="404" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="404" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A404">
         <v>28</v>
       </c>
@@ -18205,7 +18286,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="405" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="405" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A405">
         <v>28</v>
       </c>
@@ -18228,7 +18309,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="406" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="406" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A406">
         <v>28</v>
       </c>
@@ -18251,7 +18332,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="407" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="407" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A407">
         <v>29</v>
       </c>
@@ -18274,7 +18355,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="408" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="408" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A408">
         <v>29</v>
       </c>
@@ -18297,7 +18378,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="409" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="409" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A409">
         <v>29</v>
       </c>
@@ -18320,7 +18401,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="410" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="410" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A410">
         <v>29</v>
       </c>
@@ -18343,7 +18424,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="411" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="411" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A411">
         <v>29</v>
       </c>
@@ -18366,7 +18447,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="412" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="412" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A412">
         <v>29</v>
       </c>
@@ -18389,7 +18470,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="413" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="413" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A413">
         <v>29</v>
       </c>
@@ -18412,7 +18493,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="414" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="414" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A414">
         <v>29</v>
       </c>
@@ -18435,7 +18516,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="415" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="415" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A415">
         <v>29</v>
       </c>
@@ -18458,7 +18539,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="416" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="416" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A416">
         <v>29</v>
       </c>
@@ -18481,7 +18562,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="417" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A417">
         <v>29</v>
       </c>
@@ -18504,7 +18585,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="418" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="418" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A418">
         <v>29</v>
       </c>
@@ -18527,7 +18608,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="419" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="419" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A419">
         <v>29</v>
       </c>
@@ -18550,7 +18631,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="420" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="420" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A420">
         <v>29</v>
       </c>
@@ -18573,7 +18654,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="421" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="421" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A421">
         <v>29</v>
       </c>

</xml_diff>